<commit_message>
clean up code. Add input sanitization to Time class
</commit_message>
<xml_diff>
--- a/data/timeStandards/jnat-2025.xlsx
+++ b/data/timeStandards/jnat-2025.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10511"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajoe/Desktop/code/SwimDatabase/data/timeStandards/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajoe/code/swimdatabase/data/timeStandards/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484F49B4-5F13-AF4B-A5DA-E8F76C1465EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DF67CB-55C4-984C-A0E8-E7BBA3CB0612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="500" windowWidth="38280" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="199">
   <si>
     <r>
       <rPr>
@@ -1648,6 +1648,9 @@
   </si>
   <si>
     <t>3:56.29</t>
+  </si>
+  <si>
+    <t>15:34.19</t>
   </si>
 </sst>
 </file>
@@ -1978,6 +1981,99 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -1993,25 +2089,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="20"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2024,34 +2105,46 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -2101,118 +2194,28 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="8"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="9"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" indent="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="20"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1" indent="3"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="47" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -10244,239 +10247,239 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="24" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="60"/>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
+      <c r="A1" s="19"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
     </row>
     <row r="2" spans="1:19" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
       <c r="J2" s="2"/>
       <c r="K2" s="3"/>
       <c r="L2" s="4"/>
-      <c r="M2" s="82"/>
-      <c r="N2" s="82"/>
-      <c r="O2" s="82"/>
-      <c r="P2" s="82"/>
-      <c r="Q2" s="82"/>
-      <c r="R2" s="82"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
       <c r="S2" s="2"/>
     </row>
     <row r="3" spans="1:19" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="84" t="s">
+      <c r="A3" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="84"/>
-      <c r="C3" s="84"/>
-      <c r="D3" s="84"/>
-      <c r="E3" s="84"/>
-      <c r="F3" s="84"/>
-      <c r="G3" s="84"/>
-      <c r="H3" s="84"/>
-      <c r="I3" s="84"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="84"/>
-      <c r="L3" s="84"/>
-      <c r="M3" s="84"/>
-      <c r="N3" s="84"/>
-      <c r="O3" s="84"/>
-      <c r="P3" s="84"/>
-      <c r="Q3" s="84"/>
-      <c r="R3" s="84"/>
-      <c r="S3" s="84"/>
+      <c r="B3" s="22"/>
+      <c r="C3" s="22"/>
+      <c r="D3" s="22"/>
+      <c r="E3" s="22"/>
+      <c r="F3" s="22"/>
+      <c r="G3" s="22"/>
+      <c r="H3" s="22"/>
+      <c r="I3" s="22"/>
+      <c r="J3" s="22"/>
+      <c r="K3" s="22"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="22"/>
+      <c r="N3" s="22"/>
+      <c r="O3" s="22"/>
+      <c r="P3" s="22"/>
+      <c r="Q3" s="22"/>
+      <c r="R3" s="22"/>
+      <c r="S3" s="22"/>
     </row>
     <row r="4" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="60"/>
-      <c r="B4" s="60"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="85" t="s">
+      <c r="A4" s="19"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F4" s="86"/>
-      <c r="G4" s="87" t="s">
+      <c r="F4" s="24"/>
+      <c r="G4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H4" s="88"/>
-      <c r="I4" s="89"/>
-      <c r="J4" s="94" t="s">
+      <c r="H4" s="26"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="95"/>
-      <c r="L4" s="95"/>
-      <c r="M4" s="95"/>
-      <c r="N4" s="96"/>
-      <c r="O4" s="87" t="s">
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="89"/>
-      <c r="Q4" s="93" t="s">
+      <c r="P4" s="27"/>
+      <c r="Q4" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="85"/>
+      <c r="R4" s="23"/>
       <c r="S4" s="1"/>
     </row>
     <row r="5" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="60"/>
-      <c r="B5" s="60"/>
-      <c r="C5" s="60"/>
-      <c r="D5" s="60"/>
-      <c r="E5" s="61">
+      <c r="A5" s="19"/>
+      <c r="B5" s="19"/>
+      <c r="C5" s="19"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="32">
         <v>22.99</v>
       </c>
-      <c r="F5" s="62"/>
-      <c r="G5" s="73">
+      <c r="F5" s="33"/>
+      <c r="G5" s="34">
         <v>26.59</v>
       </c>
-      <c r="H5" s="74"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="24" t="s">
+      <c r="H5" s="35"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="26"/>
-      <c r="O5" s="63">
+      <c r="K5" s="38"/>
+      <c r="L5" s="38"/>
+      <c r="M5" s="38"/>
+      <c r="N5" s="39"/>
+      <c r="O5" s="40">
         <v>23.79</v>
       </c>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="63">
+      <c r="P5" s="33"/>
+      <c r="Q5" s="40">
         <v>20.39</v>
       </c>
-      <c r="R5" s="61"/>
+      <c r="R5" s="32"/>
       <c r="S5" s="1"/>
     </row>
     <row r="6" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="60"/>
-      <c r="B6" s="60"/>
-      <c r="C6" s="60"/>
-      <c r="D6" s="60"/>
-      <c r="E6" s="76">
+      <c r="A6" s="19"/>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="41">
         <v>49.99</v>
       </c>
-      <c r="F6" s="77"/>
-      <c r="G6" s="78">
+      <c r="F6" s="42"/>
+      <c r="G6" s="43">
         <v>57.69</v>
       </c>
-      <c r="H6" s="79"/>
-      <c r="I6" s="80"/>
-      <c r="J6" s="34" t="s">
+      <c r="H6" s="44"/>
+      <c r="I6" s="45"/>
+      <c r="J6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="35"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="81">
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
+      <c r="N6" s="48"/>
+      <c r="O6" s="49">
         <v>51.99</v>
       </c>
-      <c r="P6" s="77"/>
-      <c r="Q6" s="81">
+      <c r="P6" s="42"/>
+      <c r="Q6" s="49">
         <v>44.39</v>
       </c>
-      <c r="R6" s="76"/>
+      <c r="R6" s="41"/>
       <c r="S6" s="1"/>
     </row>
     <row r="7" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="60"/>
-      <c r="B7" s="60"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="19" t="s">
+      <c r="A7" s="19"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="21" t="s">
+      <c r="F7" s="51"/>
+      <c r="G7" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="22"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="24" t="s">
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
+      <c r="J7" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="21" t="s">
+      <c r="K7" s="38"/>
+      <c r="L7" s="38"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="39"/>
+      <c r="O7" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="21" t="s">
+      <c r="P7" s="54"/>
+      <c r="Q7" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="R7" s="22"/>
+      <c r="R7" s="53"/>
       <c r="S7" s="1"/>
     </row>
     <row r="8" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="60"/>
-      <c r="B8" s="60"/>
-      <c r="C8" s="60"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="43" t="s">
+      <c r="A8" s="19"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="F8" s="38"/>
-      <c r="G8" s="31" t="s">
+      <c r="F8" s="56"/>
+      <c r="G8" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="70" t="s">
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
+      <c r="J8" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="K8" s="71"/>
-      <c r="L8" s="71"/>
-      <c r="M8" s="71"/>
-      <c r="N8" s="72"/>
-      <c r="O8" s="37" t="s">
+      <c r="K8" s="61"/>
+      <c r="L8" s="61"/>
+      <c r="M8" s="61"/>
+      <c r="N8" s="62"/>
+      <c r="O8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="P8" s="38"/>
-      <c r="Q8" s="37" t="s">
+      <c r="P8" s="56"/>
+      <c r="Q8" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="R8" s="43"/>
+      <c r="R8" s="55"/>
       <c r="S8" s="1"/>
     </row>
     <row r="9" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A9" s="60"/>
-      <c r="B9" s="60"/>
-      <c r="C9" s="60"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="19" t="s">
+      <c r="A9" s="19"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="F9" s="20"/>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="51"/>
+      <c r="G9" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="22"/>
-      <c r="I9" s="23"/>
+      <c r="H9" s="53"/>
+      <c r="I9" s="54"/>
       <c r="J9" s="64" t="s">
         <v>18</v>
       </c>
@@ -10484,530 +10487,530 @@
       <c r="L9" s="65"/>
       <c r="M9" s="65"/>
       <c r="N9" s="66"/>
-      <c r="O9" s="27" t="s">
+      <c r="O9" s="67" t="s">
         <v>19</v>
       </c>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="27" t="s">
+      <c r="P9" s="51"/>
+      <c r="Q9" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="R9" s="19"/>
+      <c r="R9" s="50"/>
       <c r="S9" s="1"/>
     </row>
     <row r="10" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="60"/>
-      <c r="B10" s="60"/>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="43" t="s">
+      <c r="A10" s="19"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="38"/>
-      <c r="G10" s="31" t="s">
+      <c r="F10" s="56"/>
+      <c r="G10" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="32"/>
-      <c r="I10" s="33"/>
-      <c r="J10" s="67" t="s">
+      <c r="H10" s="58"/>
+      <c r="I10" s="59"/>
+      <c r="J10" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="68"/>
-      <c r="L10" s="68"/>
-      <c r="M10" s="68"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="31" t="s">
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="70"/>
+      <c r="O10" s="57" t="s">
         <v>24</v>
       </c>
-      <c r="P10" s="33"/>
-      <c r="Q10" s="31" t="s">
+      <c r="P10" s="59"/>
+      <c r="Q10" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="R10" s="32"/>
+      <c r="R10" s="58"/>
       <c r="S10" s="1"/>
     </row>
     <row r="11" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="60"/>
-      <c r="B11" s="60"/>
-      <c r="C11" s="60"/>
-      <c r="D11" s="60"/>
-      <c r="E11" s="61">
+      <c r="A11" s="19"/>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="32">
         <v>54.39</v>
       </c>
-      <c r="F11" s="62"/>
-      <c r="G11" s="21" t="s">
+      <c r="F11" s="33"/>
+      <c r="G11" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24" t="s">
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="63">
+      <c r="K11" s="38"/>
+      <c r="L11" s="38"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="39"/>
+      <c r="O11" s="40">
         <v>58.19</v>
       </c>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="63">
+      <c r="P11" s="33"/>
+      <c r="Q11" s="40">
         <v>48.79</v>
       </c>
-      <c r="R11" s="61"/>
+      <c r="R11" s="32"/>
       <c r="S11" s="1"/>
     </row>
     <row r="12" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="60"/>
-      <c r="B12" s="60"/>
-      <c r="C12" s="60"/>
-      <c r="D12" s="60"/>
-      <c r="E12" s="43" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="F12" s="38"/>
-      <c r="G12" s="31" t="s">
+      <c r="F12" s="56"/>
+      <c r="G12" s="57" t="s">
         <v>29</v>
       </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34" t="s">
+      <c r="H12" s="58"/>
+      <c r="I12" s="59"/>
+      <c r="J12" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="35"/>
-      <c r="L12" s="35"/>
-      <c r="M12" s="35"/>
-      <c r="N12" s="36"/>
-      <c r="O12" s="37" t="s">
+      <c r="K12" s="47"/>
+      <c r="L12" s="47"/>
+      <c r="M12" s="47"/>
+      <c r="N12" s="48"/>
+      <c r="O12" s="63" t="s">
         <v>31</v>
       </c>
-      <c r="P12" s="38"/>
-      <c r="Q12" s="31" t="s">
+      <c r="P12" s="56"/>
+      <c r="Q12" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="R12" s="32"/>
+      <c r="R12" s="58"/>
       <c r="S12" s="1"/>
     </row>
     <row r="13" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="60"/>
-      <c r="B13" s="60"/>
-      <c r="C13" s="60"/>
-      <c r="D13" s="60"/>
-      <c r="E13" s="19" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="50" t="s">
         <v>33</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="21" t="s">
+      <c r="F13" s="51"/>
+      <c r="G13" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="22"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="24" t="s">
+      <c r="H13" s="53"/>
+      <c r="I13" s="54"/>
+      <c r="J13" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="25"/>
-      <c r="M13" s="25"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="21" t="s">
+      <c r="K13" s="38"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="39"/>
+      <c r="O13" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="P13" s="23"/>
-      <c r="Q13" s="63">
+      <c r="P13" s="54"/>
+      <c r="Q13" s="40">
         <v>55.09</v>
       </c>
-      <c r="R13" s="61"/>
+      <c r="R13" s="32"/>
       <c r="S13" s="1"/>
     </row>
     <row r="14" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="60"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="43" t="s">
+      <c r="A14" s="19"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="38"/>
-      <c r="G14" s="31" t="s">
+      <c r="F14" s="56"/>
+      <c r="G14" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="32"/>
-      <c r="I14" s="33"/>
-      <c r="J14" s="34" t="s">
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
+      <c r="J14" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="K14" s="35"/>
-      <c r="L14" s="35"/>
-      <c r="M14" s="35"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="37" t="s">
+      <c r="K14" s="47"/>
+      <c r="L14" s="47"/>
+      <c r="M14" s="47"/>
+      <c r="N14" s="48"/>
+      <c r="O14" s="63" t="s">
         <v>40</v>
       </c>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="37" t="s">
+      <c r="P14" s="56"/>
+      <c r="Q14" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="R14" s="43"/>
+      <c r="R14" s="55"/>
       <c r="S14" s="1"/>
     </row>
     <row r="15" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="60"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="60"/>
-      <c r="E15" s="61">
+      <c r="A15" s="19"/>
+      <c r="B15" s="19"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="19"/>
+      <c r="E15" s="32">
         <v>54.19</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="21" t="s">
+      <c r="F15" s="33"/>
+      <c r="G15" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="H15" s="22"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24" t="s">
+      <c r="H15" s="53"/>
+      <c r="I15" s="54"/>
+      <c r="J15" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="63">
+      <c r="K15" s="38"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="39"/>
+      <c r="O15" s="40">
         <v>55.89</v>
       </c>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="63">
+      <c r="P15" s="33"/>
+      <c r="Q15" s="40">
         <v>48.29</v>
       </c>
-      <c r="R15" s="61"/>
+      <c r="R15" s="32"/>
       <c r="S15" s="1"/>
     </row>
     <row r="16" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="60"/>
-      <c r="B16" s="60"/>
-      <c r="C16" s="60"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="43" t="s">
+      <c r="A16" s="19"/>
+      <c r="B16" s="19"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="38"/>
-      <c r="G16" s="31" t="s">
+      <c r="F16" s="56"/>
+      <c r="G16" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16" s="33"/>
-      <c r="J16" s="34" t="s">
+      <c r="H16" s="58"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="36"/>
-      <c r="O16" s="37" t="s">
+      <c r="K16" s="47"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="47"/>
+      <c r="N16" s="48"/>
+      <c r="O16" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="P16" s="38"/>
-      <c r="Q16" s="31" t="s">
+      <c r="P16" s="56"/>
+      <c r="Q16" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="R16" s="32"/>
+      <c r="R16" s="58"/>
       <c r="S16" s="1"/>
     </row>
     <row r="17" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="60"/>
-      <c r="B17" s="60"/>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="19" t="s">
+      <c r="A17" s="19"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21" t="s">
+      <c r="F17" s="51"/>
+      <c r="G17" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="22"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24" t="s">
+      <c r="H17" s="53"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="K17" s="25"/>
-      <c r="L17" s="25"/>
-      <c r="M17" s="25"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="27" t="s">
+      <c r="K17" s="38"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="38"/>
+      <c r="N17" s="39"/>
+      <c r="O17" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="P17" s="20"/>
-      <c r="Q17" s="21" t="s">
+      <c r="P17" s="51"/>
+      <c r="Q17" s="52" t="s">
         <v>52</v>
       </c>
-      <c r="R17" s="22"/>
+      <c r="R17" s="53"/>
       <c r="S17" s="1"/>
     </row>
     <row r="18" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="60"/>
-      <c r="B18" s="60"/>
-      <c r="C18" s="60"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="43" t="s">
+      <c r="A18" s="19"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="F18" s="38"/>
-      <c r="G18" s="31" t="s">
+      <c r="F18" s="56"/>
+      <c r="G18" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="32"/>
-      <c r="I18" s="33"/>
-      <c r="J18" s="34" t="s">
+      <c r="H18" s="58"/>
+      <c r="I18" s="59"/>
+      <c r="J18" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-      <c r="N18" s="36"/>
-      <c r="O18" s="37" t="s">
+      <c r="K18" s="47"/>
+      <c r="L18" s="47"/>
+      <c r="M18" s="47"/>
+      <c r="N18" s="48"/>
+      <c r="O18" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="P18" s="38"/>
-      <c r="Q18" s="37" t="s">
+      <c r="P18" s="56"/>
+      <c r="Q18" s="63" t="s">
         <v>57</v>
       </c>
-      <c r="R18" s="43"/>
+      <c r="R18" s="55"/>
       <c r="S18" s="1"/>
     </row>
     <row r="19" spans="1:19" ht="298" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="20" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="60"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="60"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="60"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="60"/>
-      <c r="H20" s="60"/>
-      <c r="I20" s="60"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="60"/>
-      <c r="L20" s="60"/>
-      <c r="M20" s="60"/>
-      <c r="N20" s="60"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="60"/>
-      <c r="S20" s="60"/>
+      <c r="A20" s="19"/>
+      <c r="B20" s="19"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
     </row>
     <row r="21" spans="1:19" ht="39.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="82"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="82"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="83"/>
-      <c r="F21" s="83"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
       <c r="J21" s="2"/>
       <c r="K21" s="3"/>
       <c r="L21" s="4"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="82"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
       <c r="S21" s="2"/>
     </row>
     <row r="22" spans="1:19" ht="150" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="84" t="s">
+      <c r="A22" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="84"/>
-      <c r="C22" s="84"/>
-      <c r="D22" s="84"/>
-      <c r="E22" s="84"/>
-      <c r="F22" s="84"/>
-      <c r="G22" s="84"/>
-      <c r="H22" s="84"/>
-      <c r="I22" s="84"/>
-      <c r="J22" s="84"/>
-      <c r="K22" s="84"/>
-      <c r="L22" s="84"/>
-      <c r="M22" s="84"/>
-      <c r="N22" s="84"/>
-      <c r="O22" s="84"/>
-      <c r="P22" s="84"/>
-      <c r="Q22" s="84"/>
-      <c r="R22" s="84"/>
-      <c r="S22" s="84"/>
+      <c r="B22" s="22"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="22"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="22"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
+      <c r="J22" s="22"/>
+      <c r="K22" s="22"/>
+      <c r="L22" s="22"/>
+      <c r="M22" s="22"/>
+      <c r="N22" s="22"/>
+      <c r="O22" s="22"/>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="22"/>
+      <c r="S22" s="22"/>
     </row>
     <row r="23" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="60"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="85" t="s">
+      <c r="A23" s="19"/>
+      <c r="B23" s="19"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="19"/>
+      <c r="E23" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="F23" s="86"/>
-      <c r="G23" s="87" t="s">
+      <c r="F23" s="24"/>
+      <c r="G23" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="H23" s="88"/>
-      <c r="I23" s="89"/>
-      <c r="J23" s="90" t="s">
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
+      <c r="J23" s="71" t="s">
         <v>58</v>
       </c>
-      <c r="K23" s="91"/>
-      <c r="L23" s="91"/>
-      <c r="M23" s="91"/>
-      <c r="N23" s="92"/>
-      <c r="O23" s="87" t="s">
+      <c r="K23" s="72"/>
+      <c r="L23" s="72"/>
+      <c r="M23" s="72"/>
+      <c r="N23" s="73"/>
+      <c r="O23" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P23" s="89"/>
-      <c r="Q23" s="93" t="s">
+      <c r="P23" s="27"/>
+      <c r="Q23" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="R23" s="85"/>
+      <c r="R23" s="23"/>
       <c r="S23" s="1"/>
     </row>
     <row r="24" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="60"/>
-      <c r="B24" s="60"/>
-      <c r="C24" s="60"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="61">
+      <c r="A24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="32">
         <v>23.29</v>
       </c>
-      <c r="F24" s="62"/>
-      <c r="G24" s="73">
+      <c r="F24" s="33"/>
+      <c r="G24" s="34">
         <v>26.89</v>
       </c>
-      <c r="H24" s="74"/>
-      <c r="I24" s="75"/>
-      <c r="J24" s="24" t="s">
+      <c r="H24" s="35"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="25"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="63">
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="38"/>
+      <c r="N24" s="39"/>
+      <c r="O24" s="40">
         <v>24.09</v>
       </c>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="63">
+      <c r="P24" s="33"/>
+      <c r="Q24" s="40">
         <v>20.59</v>
       </c>
-      <c r="R24" s="61"/>
+      <c r="R24" s="32"/>
       <c r="S24" s="1"/>
     </row>
     <row r="25" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="60"/>
-      <c r="B25" s="60"/>
-      <c r="C25" s="60"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="76">
+      <c r="A25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="41">
         <v>50.39</v>
       </c>
-      <c r="F25" s="77"/>
-      <c r="G25" s="78">
+      <c r="F25" s="42"/>
+      <c r="G25" s="43">
         <v>58.19</v>
       </c>
-      <c r="H25" s="79"/>
-      <c r="I25" s="80"/>
-      <c r="J25" s="34" t="s">
+      <c r="H25" s="44"/>
+      <c r="I25" s="45"/>
+      <c r="J25" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="K25" s="35"/>
-      <c r="L25" s="35"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="36"/>
-      <c r="O25" s="81">
+      <c r="K25" s="47"/>
+      <c r="L25" s="47"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="48"/>
+      <c r="O25" s="49">
         <v>52.59</v>
       </c>
-      <c r="P25" s="77"/>
-      <c r="Q25" s="81">
+      <c r="P25" s="42"/>
+      <c r="Q25" s="49">
         <v>44.99</v>
       </c>
-      <c r="R25" s="76"/>
+      <c r="R25" s="41"/>
       <c r="S25" s="1"/>
     </row>
     <row r="26" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="60"/>
-      <c r="B26" s="60"/>
-      <c r="C26" s="60"/>
-      <c r="D26" s="60"/>
-      <c r="E26" s="19" t="s">
+      <c r="A26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="19"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="50" t="s">
         <v>59</v>
       </c>
-      <c r="F26" s="20"/>
-      <c r="G26" s="21" t="s">
+      <c r="F26" s="51"/>
+      <c r="G26" s="52" t="s">
         <v>7</v>
       </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24" t="s">
+      <c r="H26" s="53"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="K26" s="25"/>
-      <c r="L26" s="25"/>
-      <c r="M26" s="25"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="21" t="s">
+      <c r="K26" s="38"/>
+      <c r="L26" s="38"/>
+      <c r="M26" s="38"/>
+      <c r="N26" s="39"/>
+      <c r="O26" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="21" t="s">
+      <c r="P26" s="54"/>
+      <c r="Q26" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="R26" s="22"/>
+      <c r="R26" s="53"/>
       <c r="S26" s="1"/>
     </row>
     <row r="27" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="60"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="43" t="s">
+      <c r="A27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="55" t="s">
         <v>62</v>
       </c>
-      <c r="F27" s="38"/>
-      <c r="G27" s="31" t="s">
+      <c r="F27" s="56"/>
+      <c r="G27" s="57" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="32"/>
-      <c r="I27" s="33"/>
-      <c r="J27" s="70" t="s">
+      <c r="H27" s="58"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="71"/>
-      <c r="L27" s="71"/>
-      <c r="M27" s="71"/>
-      <c r="N27" s="72"/>
-      <c r="O27" s="37" t="s">
+      <c r="K27" s="61"/>
+      <c r="L27" s="61"/>
+      <c r="M27" s="61"/>
+      <c r="N27" s="62"/>
+      <c r="O27" s="63" t="s">
         <v>64</v>
       </c>
-      <c r="P27" s="38"/>
-      <c r="Q27" s="37" t="s">
+      <c r="P27" s="56"/>
+      <c r="Q27" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="R27" s="43"/>
+      <c r="R27" s="55"/>
       <c r="S27" s="1"/>
     </row>
     <row r="28" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="60"/>
-      <c r="B28" s="60"/>
-      <c r="C28" s="60"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="19" t="s">
+      <c r="A28" s="19"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="50" t="s">
         <v>66</v>
       </c>
-      <c r="F28" s="20"/>
-      <c r="G28" s="21" t="s">
+      <c r="F28" s="51"/>
+      <c r="G28" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="23"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="54"/>
       <c r="J28" s="64" t="s">
         <v>18</v>
       </c>
@@ -11015,795 +11018,577 @@
       <c r="L28" s="65"/>
       <c r="M28" s="65"/>
       <c r="N28" s="66"/>
-      <c r="O28" s="27" t="s">
+      <c r="O28" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="P28" s="20"/>
-      <c r="Q28" s="27" t="s">
+      <c r="P28" s="51"/>
+      <c r="Q28" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="R28" s="19"/>
+      <c r="R28" s="50"/>
       <c r="S28" s="1"/>
     </row>
     <row r="29" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="60"/>
-      <c r="B29" s="60"/>
-      <c r="C29" s="60"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="43" t="s">
+      <c r="A29" s="19"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="19"/>
+      <c r="E29" s="55" t="s">
         <v>69</v>
       </c>
-      <c r="F29" s="38"/>
-      <c r="G29" s="31" t="s">
+      <c r="F29" s="56"/>
+      <c r="G29" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="H29" s="32"/>
-      <c r="I29" s="33"/>
-      <c r="J29" s="67" t="s">
+      <c r="H29" s="58"/>
+      <c r="I29" s="59"/>
+      <c r="J29" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="K29" s="68"/>
-      <c r="L29" s="68"/>
-      <c r="M29" s="68"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="31" t="s">
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="70"/>
+      <c r="O29" s="57" t="s">
         <v>70</v>
       </c>
-      <c r="P29" s="33"/>
-      <c r="Q29" s="31" t="s">
+      <c r="P29" s="59"/>
+      <c r="Q29" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="R29" s="32"/>
+      <c r="R29" s="58"/>
       <c r="S29" s="1"/>
     </row>
     <row r="30" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="60"/>
-      <c r="B30" s="60"/>
-      <c r="C30" s="60"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="61">
+      <c r="A30" s="19"/>
+      <c r="B30" s="19"/>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="32">
         <v>55.09</v>
       </c>
-      <c r="F30" s="62"/>
-      <c r="G30" s="21" t="s">
+      <c r="F30" s="33"/>
+      <c r="G30" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="22"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="24" t="s">
+      <c r="H30" s="53"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="K30" s="25"/>
-      <c r="L30" s="25"/>
-      <c r="M30" s="25"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="63">
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="38"/>
+      <c r="N30" s="39"/>
+      <c r="O30" s="40">
         <v>58.79</v>
       </c>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="63">
+      <c r="P30" s="33"/>
+      <c r="Q30" s="40">
         <v>49.29</v>
       </c>
-      <c r="R30" s="61"/>
+      <c r="R30" s="32"/>
       <c r="S30" s="1"/>
     </row>
     <row r="31" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="60"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="60"/>
-      <c r="E31" s="43" t="s">
+      <c r="A31" s="19"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="19"/>
+      <c r="D31" s="19"/>
+      <c r="E31" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="F31" s="38"/>
-      <c r="G31" s="31" t="s">
+      <c r="F31" s="56"/>
+      <c r="G31" s="57" t="s">
         <v>74</v>
       </c>
-      <c r="H31" s="32"/>
-      <c r="I31" s="33"/>
-      <c r="J31" s="34" t="s">
+      <c r="H31" s="58"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="K31" s="35"/>
-      <c r="L31" s="35"/>
-      <c r="M31" s="35"/>
-      <c r="N31" s="36"/>
-      <c r="O31" s="37" t="s">
+      <c r="K31" s="47"/>
+      <c r="L31" s="47"/>
+      <c r="M31" s="47"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="P31" s="38"/>
-      <c r="Q31" s="31" t="s">
+      <c r="P31" s="56"/>
+      <c r="Q31" s="57" t="s">
         <v>76</v>
       </c>
-      <c r="R31" s="32"/>
+      <c r="R31" s="58"/>
       <c r="S31" s="1"/>
     </row>
     <row r="32" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="60"/>
-      <c r="B32" s="60"/>
-      <c r="C32" s="60"/>
-      <c r="D32" s="60"/>
-      <c r="E32" s="19" t="s">
+      <c r="A32" s="19"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="50" t="s">
         <v>77</v>
       </c>
-      <c r="F32" s="20"/>
-      <c r="G32" s="21" t="s">
+      <c r="F32" s="51"/>
+      <c r="G32" s="52" t="s">
         <v>78</v>
       </c>
-      <c r="H32" s="22"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="24" t="s">
+      <c r="H32" s="53"/>
+      <c r="I32" s="54"/>
+      <c r="J32" s="37" t="s">
         <v>35</v>
       </c>
-      <c r="K32" s="25"/>
-      <c r="L32" s="25"/>
-      <c r="M32" s="25"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="21" t="s">
+      <c r="K32" s="38"/>
+      <c r="L32" s="38"/>
+      <c r="M32" s="38"/>
+      <c r="N32" s="39"/>
+      <c r="O32" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="P32" s="23"/>
-      <c r="Q32" s="63">
+      <c r="P32" s="54"/>
+      <c r="Q32" s="40">
         <v>55.69</v>
       </c>
-      <c r="R32" s="61"/>
+      <c r="R32" s="32"/>
       <c r="S32" s="1"/>
     </row>
     <row r="33" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="60"/>
-      <c r="B33" s="60"/>
-      <c r="C33" s="60"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="43" t="s">
+      <c r="A33" s="19"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
+      <c r="D33" s="19"/>
+      <c r="E33" s="55" t="s">
         <v>80</v>
       </c>
-      <c r="F33" s="38"/>
-      <c r="G33" s="31" t="s">
+      <c r="F33" s="56"/>
+      <c r="G33" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="H33" s="32"/>
-      <c r="I33" s="33"/>
-      <c r="J33" s="34" t="s">
+      <c r="H33" s="58"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="K33" s="35"/>
-      <c r="L33" s="35"/>
-      <c r="M33" s="35"/>
-      <c r="N33" s="36"/>
-      <c r="O33" s="37" t="s">
+      <c r="K33" s="47"/>
+      <c r="L33" s="47"/>
+      <c r="M33" s="47"/>
+      <c r="N33" s="48"/>
+      <c r="O33" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="37" t="s">
+      <c r="P33" s="56"/>
+      <c r="Q33" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="R33" s="43"/>
+      <c r="R33" s="55"/>
       <c r="S33" s="1"/>
     </row>
     <row r="34" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="60"/>
-      <c r="B34" s="60"/>
-      <c r="C34" s="60"/>
-      <c r="D34" s="60"/>
-      <c r="E34" s="61">
+      <c r="A34" s="19"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="32">
         <v>54.69</v>
       </c>
-      <c r="F34" s="62"/>
-      <c r="G34" s="21" t="s">
+      <c r="F34" s="33"/>
+      <c r="G34" s="52" t="s">
         <v>83</v>
       </c>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="24" t="s">
+      <c r="H34" s="53"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="37" t="s">
         <v>43</v>
       </c>
-      <c r="K34" s="25"/>
-      <c r="L34" s="25"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="63">
+      <c r="K34" s="38"/>
+      <c r="L34" s="38"/>
+      <c r="M34" s="38"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="40">
         <v>56.59</v>
       </c>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="63">
+      <c r="P34" s="33"/>
+      <c r="Q34" s="40">
         <v>48.79</v>
       </c>
-      <c r="R34" s="61"/>
+      <c r="R34" s="32"/>
       <c r="S34" s="1"/>
     </row>
     <row r="35" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="60"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="43" t="s">
+      <c r="A35" s="19"/>
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="19"/>
+      <c r="E35" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="F35" s="38"/>
-      <c r="G35" s="31" t="s">
+      <c r="F35" s="56"/>
+      <c r="G35" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="H35" s="32"/>
-      <c r="I35" s="33"/>
-      <c r="J35" s="34" t="s">
+      <c r="H35" s="58"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="K35" s="35"/>
-      <c r="L35" s="35"/>
-      <c r="M35" s="35"/>
-      <c r="N35" s="36"/>
-      <c r="O35" s="37" t="s">
+      <c r="K35" s="47"/>
+      <c r="L35" s="47"/>
+      <c r="M35" s="47"/>
+      <c r="N35" s="48"/>
+      <c r="O35" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="P35" s="38"/>
-      <c r="Q35" s="31" t="s">
+      <c r="P35" s="56"/>
+      <c r="Q35" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="R35" s="32"/>
+      <c r="R35" s="58"/>
       <c r="S35" s="1"/>
     </row>
     <row r="36" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A36" s="60"/>
-      <c r="B36" s="60"/>
-      <c r="C36" s="60"/>
-      <c r="D36" s="60"/>
-      <c r="E36" s="19" t="s">
+      <c r="A36" s="19"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="19"/>
+      <c r="E36" s="50" t="s">
         <v>87</v>
       </c>
-      <c r="F36" s="20"/>
-      <c r="G36" s="21" t="s">
+      <c r="F36" s="51"/>
+      <c r="G36" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="24" t="s">
+      <c r="H36" s="53"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="37" t="s">
         <v>50</v>
       </c>
-      <c r="K36" s="25"/>
-      <c r="L36" s="25"/>
-      <c r="M36" s="25"/>
-      <c r="N36" s="26"/>
-      <c r="O36" s="27" t="s">
+      <c r="K36" s="38"/>
+      <c r="L36" s="38"/>
+      <c r="M36" s="38"/>
+      <c r="N36" s="39"/>
+      <c r="O36" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="P36" s="20"/>
-      <c r="Q36" s="21" t="s">
+      <c r="P36" s="51"/>
+      <c r="Q36" s="52" t="s">
         <v>90</v>
       </c>
-      <c r="R36" s="22"/>
+      <c r="R36" s="53"/>
       <c r="S36" s="1"/>
     </row>
     <row r="37" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A37" s="60"/>
-      <c r="B37" s="60"/>
-      <c r="C37" s="60"/>
-      <c r="D37" s="60"/>
-      <c r="E37" s="43" t="s">
+      <c r="A37" s="19"/>
+      <c r="B37" s="19"/>
+      <c r="C37" s="19"/>
+      <c r="D37" s="19"/>
+      <c r="E37" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="F37" s="38"/>
-      <c r="G37" s="31" t="s">
+      <c r="F37" s="56"/>
+      <c r="G37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="H37" s="32"/>
-      <c r="I37" s="33"/>
-      <c r="J37" s="34" t="s">
+      <c r="H37" s="58"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="K37" s="35"/>
-      <c r="L37" s="35"/>
-      <c r="M37" s="35"/>
-      <c r="N37" s="36"/>
-      <c r="O37" s="37" t="s">
+      <c r="K37" s="47"/>
+      <c r="L37" s="47"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="48"/>
+      <c r="O37" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="P37" s="38"/>
-      <c r="Q37" s="37" t="s">
+      <c r="P37" s="56"/>
+      <c r="Q37" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="R37" s="43"/>
+      <c r="R37" s="55"/>
       <c r="S37" s="1"/>
     </row>
     <row r="38" spans="1:19" ht="298" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="39" spans="1:19" ht="139.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A39" s="44" t="s">
+      <c r="A39" s="74" t="s">
         <v>94</v>
       </c>
-      <c r="B39" s="44"/>
-      <c r="C39" s="44"/>
-      <c r="D39" s="44"/>
-      <c r="E39" s="44"/>
-      <c r="F39" s="44"/>
-      <c r="G39" s="44"/>
-      <c r="H39" s="45" t="s">
+      <c r="B39" s="74"/>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="75" t="s">
         <v>95</v>
       </c>
-      <c r="I39" s="45"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="45"/>
-      <c r="M39" s="45"/>
-      <c r="N39" s="45"/>
-      <c r="O39" s="45"/>
-      <c r="P39" s="45"/>
-      <c r="Q39" s="45"/>
-      <c r="R39" s="45"/>
-      <c r="S39" s="45"/>
+      <c r="I39" s="75"/>
+      <c r="J39" s="75"/>
+      <c r="K39" s="75"/>
+      <c r="L39" s="75"/>
+      <c r="M39" s="75"/>
+      <c r="N39" s="75"/>
+      <c r="O39" s="75"/>
+      <c r="P39" s="75"/>
+      <c r="Q39" s="75"/>
+      <c r="R39" s="75"/>
+      <c r="S39" s="75"/>
     </row>
     <row r="40" spans="1:19" ht="39" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="5"/>
-      <c r="B40" s="46"/>
-      <c r="C40" s="47"/>
+      <c r="B40" s="76"/>
+      <c r="C40" s="77"/>
     </row>
     <row r="41" spans="1:19" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="48"/>
-      <c r="B41" s="49"/>
+      <c r="A41" s="78"/>
+      <c r="B41" s="79"/>
     </row>
     <row r="42" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="48"/>
-      <c r="B42" s="49"/>
+      <c r="A42" s="78"/>
+      <c r="B42" s="79"/>
     </row>
     <row r="43" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="50" t="s">
+      <c r="A43" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B43" s="50"/>
-      <c r="C43" s="50"/>
-      <c r="D43" s="50"/>
-      <c r="E43" s="50"/>
-      <c r="F43" s="50"/>
-      <c r="G43" s="50"/>
-      <c r="H43" s="50"/>
-      <c r="I43" s="50"/>
-      <c r="J43" s="50"/>
-      <c r="K43" s="50"/>
-      <c r="L43" s="50"/>
-      <c r="M43" s="50"/>
-      <c r="N43" s="50"/>
-      <c r="O43" s="50"/>
-      <c r="P43" s="50"/>
-      <c r="Q43" s="50"/>
-      <c r="R43" s="50"/>
-      <c r="S43" s="50"/>
+      <c r="B43" s="80"/>
+      <c r="C43" s="80"/>
+      <c r="D43" s="80"/>
+      <c r="E43" s="80"/>
+      <c r="F43" s="80"/>
+      <c r="G43" s="80"/>
+      <c r="H43" s="80"/>
+      <c r="I43" s="80"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80"/>
+      <c r="M43" s="80"/>
+      <c r="N43" s="80"/>
+      <c r="O43" s="80"/>
+      <c r="P43" s="80"/>
+      <c r="Q43" s="80"/>
+      <c r="R43" s="80"/>
+      <c r="S43" s="80"/>
     </row>
     <row r="44" spans="1:19" ht="133.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A44" s="51"/>
-      <c r="B44" s="51"/>
-      <c r="C44" s="51"/>
-      <c r="D44" s="51"/>
-      <c r="E44" s="51"/>
-      <c r="F44" s="51"/>
-      <c r="G44" s="51"/>
-      <c r="H44" s="51"/>
-      <c r="I44" s="51"/>
-      <c r="J44" s="51"/>
-      <c r="K44" s="51"/>
-      <c r="L44" s="51"/>
-      <c r="M44" s="51"/>
-      <c r="N44" s="51"/>
-      <c r="O44" s="51"/>
-      <c r="P44" s="51"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="51"/>
-      <c r="S44" s="51"/>
+      <c r="A44" s="81"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="81"/>
+      <c r="D44" s="81"/>
+      <c r="E44" s="81"/>
+      <c r="F44" s="81"/>
+      <c r="G44" s="81"/>
+      <c r="H44" s="81"/>
+      <c r="I44" s="81"/>
+      <c r="J44" s="81"/>
+      <c r="K44" s="81"/>
+      <c r="L44" s="81"/>
+      <c r="M44" s="81"/>
+      <c r="N44" s="81"/>
+      <c r="O44" s="81"/>
+      <c r="P44" s="81"/>
+      <c r="Q44" s="81"/>
+      <c r="R44" s="81"/>
+      <c r="S44" s="81"/>
     </row>
     <row r="45" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="52" t="s">
+      <c r="A45" s="82" t="s">
         <v>96</v>
       </c>
-      <c r="B45" s="52"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="52"/>
-      <c r="E45" s="53"/>
-      <c r="F45" s="54" t="s">
+      <c r="B45" s="82"/>
+      <c r="C45" s="82"/>
+      <c r="D45" s="82"/>
+      <c r="E45" s="83"/>
+      <c r="F45" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="G45" s="55"/>
-      <c r="H45" s="56"/>
-      <c r="I45" s="57" t="s">
+      <c r="G45" s="85"/>
+      <c r="H45" s="86"/>
+      <c r="I45" s="87" t="s">
         <v>98</v>
       </c>
-      <c r="J45" s="58"/>
-      <c r="K45" s="58"/>
-      <c r="L45" s="58"/>
-      <c r="M45" s="59"/>
-      <c r="N45" s="54" t="s">
+      <c r="J45" s="88"/>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
+      <c r="M45" s="89"/>
+      <c r="N45" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="O45" s="56"/>
-      <c r="P45" s="54" t="s">
+      <c r="O45" s="86"/>
+      <c r="P45" s="84" t="s">
         <v>96</v>
       </c>
-      <c r="Q45" s="55"/>
+      <c r="Q45" s="85"/>
     </row>
     <row r="46" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="40" t="s">
+      <c r="A46" s="90" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="40"/>
-      <c r="E46" s="41"/>
-      <c r="F46" s="21" t="s">
+      <c r="B46" s="90"/>
+      <c r="C46" s="90"/>
+      <c r="D46" s="90"/>
+      <c r="E46" s="91"/>
+      <c r="F46" s="52" t="s">
         <v>100</v>
       </c>
-      <c r="G46" s="22"/>
-      <c r="H46" s="23"/>
-      <c r="I46" s="24" t="s">
+      <c r="G46" s="53"/>
+      <c r="H46" s="54"/>
+      <c r="I46" s="37" t="s">
         <v>101</v>
       </c>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="27" t="s">
+      <c r="J46" s="38"/>
+      <c r="K46" s="38"/>
+      <c r="L46" s="38"/>
+      <c r="M46" s="39"/>
+      <c r="N46" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="O46" s="20"/>
-      <c r="P46" s="42" t="s">
+      <c r="O46" s="51"/>
+      <c r="P46" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="Q46" s="40"/>
+      <c r="Q46" s="90"/>
     </row>
     <row r="47" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="43" t="s">
+      <c r="A47" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="43"/>
-      <c r="E47" s="38"/>
-      <c r="F47" s="31" t="s">
+      <c r="B47" s="55"/>
+      <c r="C47" s="55"/>
+      <c r="D47" s="55"/>
+      <c r="E47" s="56"/>
+      <c r="F47" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="G47" s="32"/>
-      <c r="H47" s="33"/>
-      <c r="I47" s="34" t="s">
+      <c r="G47" s="58"/>
+      <c r="H47" s="59"/>
+      <c r="I47" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="J47" s="35"/>
-      <c r="K47" s="35"/>
-      <c r="L47" s="35"/>
-      <c r="M47" s="36"/>
-      <c r="N47" s="37" t="s">
+      <c r="J47" s="47"/>
+      <c r="K47" s="47"/>
+      <c r="L47" s="47"/>
+      <c r="M47" s="48"/>
+      <c r="N47" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="O47" s="38"/>
-      <c r="P47" s="37" t="s">
+      <c r="O47" s="56"/>
+      <c r="P47" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="Q47" s="43"/>
+      <c r="Q47" s="55"/>
     </row>
     <row r="48" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="50" t="s">
         <v>106</v>
       </c>
-      <c r="B48" s="19"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="19"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="21" t="s">
+      <c r="B48" s="50"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="51"/>
+      <c r="F48" s="52" t="s">
         <v>107</v>
       </c>
-      <c r="G48" s="22"/>
-      <c r="H48" s="23"/>
-      <c r="I48" s="24" t="s">
+      <c r="G48" s="53"/>
+      <c r="H48" s="54"/>
+      <c r="I48" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="21" t="s">
+      <c r="J48" s="38"/>
+      <c r="K48" s="38"/>
+      <c r="L48" s="38"/>
+      <c r="M48" s="39"/>
+      <c r="N48" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="O48" s="23"/>
-      <c r="P48" s="27" t="s">
+      <c r="O48" s="54"/>
+      <c r="P48" s="67" t="s">
         <v>110</v>
       </c>
-      <c r="Q48" s="19"/>
+      <c r="Q48" s="50"/>
     </row>
     <row r="49" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="94" t="s">
         <v>99</v>
       </c>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="30"/>
-      <c r="F49" s="31" t="s">
+      <c r="B49" s="94"/>
+      <c r="C49" s="94"/>
+      <c r="D49" s="94"/>
+      <c r="E49" s="95"/>
+      <c r="F49" s="57" t="s">
         <v>111</v>
       </c>
-      <c r="G49" s="32"/>
-      <c r="H49" s="33"/>
-      <c r="I49" s="34" t="s">
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="46" t="s">
         <v>112</v>
       </c>
-      <c r="J49" s="35"/>
-      <c r="K49" s="35"/>
-      <c r="L49" s="35"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="37" t="s">
+      <c r="J49" s="47"/>
+      <c r="K49" s="47"/>
+      <c r="L49" s="47"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="O49" s="38"/>
-      <c r="P49" s="39" t="s">
+      <c r="O49" s="56"/>
+      <c r="P49" s="96" t="s">
         <v>99</v>
       </c>
-      <c r="Q49" s="29"/>
+      <c r="Q49" s="94"/>
     </row>
     <row r="50" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="50" t="s">
         <v>114</v>
       </c>
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="21" t="s">
+      <c r="B50" s="50"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="50"/>
+      <c r="E50" s="51"/>
+      <c r="F50" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="G50" s="22"/>
-      <c r="H50" s="23"/>
-      <c r="I50" s="24" t="s">
+      <c r="G50" s="53"/>
+      <c r="H50" s="54"/>
+      <c r="I50" s="37" t="s">
         <v>115</v>
       </c>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="27" t="s">
+      <c r="J50" s="38"/>
+      <c r="K50" s="38"/>
+      <c r="L50" s="38"/>
+      <c r="M50" s="39"/>
+      <c r="N50" s="67" t="s">
         <v>113</v>
       </c>
-      <c r="O50" s="20"/>
-      <c r="P50" s="27" t="s">
+      <c r="O50" s="51"/>
+      <c r="P50" s="67" t="s">
         <v>116</v>
       </c>
-      <c r="Q50" s="19"/>
+      <c r="Q50" s="50"/>
     </row>
     <row r="51" spans="1:19" ht="62.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="93" t="s">
         <v>117</v>
       </c>
-      <c r="B51" s="28"/>
-      <c r="C51" s="28"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="28"/>
-      <c r="G51" s="28"/>
-      <c r="H51" s="28"/>
-      <c r="I51" s="28"/>
-      <c r="J51" s="28"/>
-      <c r="K51" s="28"/>
-      <c r="L51" s="28"/>
-      <c r="M51" s="28"/>
-      <c r="N51" s="28"/>
-      <c r="O51" s="28"/>
-      <c r="P51" s="28"/>
-      <c r="Q51" s="28"/>
-      <c r="R51" s="28"/>
-      <c r="S51" s="28"/>
+      <c r="B51" s="93"/>
+      <c r="C51" s="93"/>
+      <c r="D51" s="93"/>
+      <c r="E51" s="93"/>
+      <c r="F51" s="93"/>
+      <c r="G51" s="93"/>
+      <c r="H51" s="93"/>
+      <c r="I51" s="93"/>
+      <c r="J51" s="93"/>
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
+      <c r="M51" s="93"/>
+      <c r="N51" s="93"/>
+      <c r="O51" s="93"/>
+      <c r="P51" s="93"/>
+      <c r="Q51" s="93"/>
+      <c r="R51" s="93"/>
+      <c r="S51" s="93"/>
     </row>
   </sheetData>
   <mergeCells count="234">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:I2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="A3:S3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:N5"/>
-    <mergeCell ref="O5:P5"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="G6:I6"/>
-    <mergeCell ref="J6:N6"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="Q6:R6"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="G7:I7"/>
-    <mergeCell ref="J7:N7"/>
-    <mergeCell ref="O7:P7"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:I8"/>
-    <mergeCell ref="J8:N8"/>
-    <mergeCell ref="O8:P8"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="G9:I9"/>
-    <mergeCell ref="J9:N9"/>
-    <mergeCell ref="O9:P9"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="G10:I10"/>
-    <mergeCell ref="J10:N10"/>
-    <mergeCell ref="O10:P10"/>
-    <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:I11"/>
-    <mergeCell ref="J11:N11"/>
-    <mergeCell ref="O11:P11"/>
-    <mergeCell ref="Q11:R11"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="E12:F12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="J12:N12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="A13:D13"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="G13:I13"/>
-    <mergeCell ref="J13:N13"/>
-    <mergeCell ref="O13:P13"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="G14:I14"/>
-    <mergeCell ref="J14:N14"/>
-    <mergeCell ref="O14:P14"/>
-    <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="A15:D15"/>
-    <mergeCell ref="E15:F15"/>
-    <mergeCell ref="G15:I15"/>
-    <mergeCell ref="J15:N15"/>
-    <mergeCell ref="O15:P15"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="J16:N16"/>
-    <mergeCell ref="O16:P16"/>
-    <mergeCell ref="Q16:R16"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:N17"/>
-    <mergeCell ref="O17:P17"/>
-    <mergeCell ref="Q17:R17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="J18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="Q18:R18"/>
-    <mergeCell ref="A20:S20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="M21:N21"/>
-    <mergeCell ref="O21:P21"/>
-    <mergeCell ref="Q21:R21"/>
-    <mergeCell ref="A22:S22"/>
-    <mergeCell ref="A23:D23"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="G23:I23"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="O23:P23"/>
-    <mergeCell ref="Q23:R23"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="E24:F24"/>
-    <mergeCell ref="G24:I24"/>
-    <mergeCell ref="J24:N24"/>
-    <mergeCell ref="O24:P24"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="A25:D25"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:N25"/>
-    <mergeCell ref="O25:P25"/>
-    <mergeCell ref="Q25:R25"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="G26:I26"/>
-    <mergeCell ref="J26:N26"/>
-    <mergeCell ref="O26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="A27:D27"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J27:N27"/>
-    <mergeCell ref="O27:P27"/>
-    <mergeCell ref="Q27:R27"/>
-    <mergeCell ref="A28:D28"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:N28"/>
-    <mergeCell ref="O28:P28"/>
-    <mergeCell ref="Q28:R28"/>
-    <mergeCell ref="A29:D29"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:N29"/>
-    <mergeCell ref="O29:P29"/>
-    <mergeCell ref="Q29:R29"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="O30:P30"/>
-    <mergeCell ref="Q30:R30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G31:I31"/>
-    <mergeCell ref="J31:N31"/>
-    <mergeCell ref="O31:P31"/>
-    <mergeCell ref="Q31:R31"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:N32"/>
-    <mergeCell ref="O32:P32"/>
-    <mergeCell ref="Q32:R32"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="J33:N33"/>
-    <mergeCell ref="O33:P33"/>
-    <mergeCell ref="Q33:R33"/>
-    <mergeCell ref="A34:D34"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:N34"/>
-    <mergeCell ref="O34:P34"/>
-    <mergeCell ref="Q34:R34"/>
-    <mergeCell ref="A35:D35"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="G35:I35"/>
-    <mergeCell ref="J35:N35"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="Q35:R35"/>
-    <mergeCell ref="A36:D36"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:N36"/>
-    <mergeCell ref="O36:P36"/>
-    <mergeCell ref="Q36:R36"/>
-    <mergeCell ref="A37:D37"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="J37:N37"/>
-    <mergeCell ref="O37:P37"/>
-    <mergeCell ref="Q37:R37"/>
-    <mergeCell ref="A39:G39"/>
-    <mergeCell ref="H39:S39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="A41:B41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A43:S43"/>
-    <mergeCell ref="A44:S44"/>
-    <mergeCell ref="A45:E45"/>
-    <mergeCell ref="F45:H45"/>
-    <mergeCell ref="I45:M45"/>
-    <mergeCell ref="N45:O45"/>
-    <mergeCell ref="P45:Q45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="F46:H46"/>
-    <mergeCell ref="I46:M46"/>
-    <mergeCell ref="N46:O46"/>
-    <mergeCell ref="P46:Q46"/>
-    <mergeCell ref="A47:E47"/>
-    <mergeCell ref="F47:H47"/>
-    <mergeCell ref="I47:M47"/>
-    <mergeCell ref="N47:O47"/>
-    <mergeCell ref="P47:Q47"/>
     <mergeCell ref="A50:E50"/>
     <mergeCell ref="F50:H50"/>
     <mergeCell ref="I50:M50"/>
@@ -11820,6 +11605,224 @@
     <mergeCell ref="I49:M49"/>
     <mergeCell ref="N49:O49"/>
     <mergeCell ref="P49:Q49"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="F46:H46"/>
+    <mergeCell ref="I46:M46"/>
+    <mergeCell ref="N46:O46"/>
+    <mergeCell ref="P46:Q46"/>
+    <mergeCell ref="A47:E47"/>
+    <mergeCell ref="F47:H47"/>
+    <mergeCell ref="I47:M47"/>
+    <mergeCell ref="N47:O47"/>
+    <mergeCell ref="P47:Q47"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="H39:S39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A43:S43"/>
+    <mergeCell ref="A44:S44"/>
+    <mergeCell ref="A45:E45"/>
+    <mergeCell ref="F45:H45"/>
+    <mergeCell ref="I45:M45"/>
+    <mergeCell ref="N45:O45"/>
+    <mergeCell ref="P45:Q45"/>
+    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:N36"/>
+    <mergeCell ref="O36:P36"/>
+    <mergeCell ref="Q36:R36"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="J37:N37"/>
+    <mergeCell ref="O37:P37"/>
+    <mergeCell ref="Q37:R37"/>
+    <mergeCell ref="A34:D34"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:N34"/>
+    <mergeCell ref="O34:P34"/>
+    <mergeCell ref="Q34:R34"/>
+    <mergeCell ref="A35:D35"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="G35:I35"/>
+    <mergeCell ref="J35:N35"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="Q35:R35"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="O32:P32"/>
+    <mergeCell ref="Q32:R32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="J33:N33"/>
+    <mergeCell ref="O33:P33"/>
+    <mergeCell ref="Q33:R33"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:N30"/>
+    <mergeCell ref="O30:P30"/>
+    <mergeCell ref="Q30:R30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G31:I31"/>
+    <mergeCell ref="J31:N31"/>
+    <mergeCell ref="O31:P31"/>
+    <mergeCell ref="Q31:R31"/>
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:N28"/>
+    <mergeCell ref="O28:P28"/>
+    <mergeCell ref="Q28:R28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:N29"/>
+    <mergeCell ref="O29:P29"/>
+    <mergeCell ref="Q29:R29"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="G26:I26"/>
+    <mergeCell ref="J26:N26"/>
+    <mergeCell ref="O26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="A27:D27"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J27:N27"/>
+    <mergeCell ref="O27:P27"/>
+    <mergeCell ref="Q27:R27"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="G24:I24"/>
+    <mergeCell ref="J24:N24"/>
+    <mergeCell ref="O24:P24"/>
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:F25"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="J25:N25"/>
+    <mergeCell ref="O25:P25"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="A20:S20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="M21:N21"/>
+    <mergeCell ref="O21:P21"/>
+    <mergeCell ref="Q21:R21"/>
+    <mergeCell ref="A22:S22"/>
+    <mergeCell ref="A23:D23"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="G23:I23"/>
+    <mergeCell ref="J23:N23"/>
+    <mergeCell ref="O23:P23"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="J17:N17"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="J18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="A15:D15"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:N15"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="J16:N16"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:I13"/>
+    <mergeCell ref="J13:N13"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="G14:I14"/>
+    <mergeCell ref="J14:N14"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:I11"/>
+    <mergeCell ref="J11:N11"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="G12:I12"/>
+    <mergeCell ref="J12:N12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="J9:N9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="G10:I10"/>
+    <mergeCell ref="J10:N10"/>
+    <mergeCell ref="O10:P10"/>
+    <mergeCell ref="Q10:R10"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="J7:N7"/>
+    <mergeCell ref="O7:P7"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="J8:N8"/>
+    <mergeCell ref="O8:P8"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:N5"/>
+    <mergeCell ref="O5:P5"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="J6:N6"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="Q6:R6"/>
+    <mergeCell ref="A1:S1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:I2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A3:S3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:N4"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="Q4:R4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11831,7 +11834,7 @@
   <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -11965,8 +11968,8 @@
         <v>171</v>
       </c>
       <c r="D7" s="18"/>
-      <c r="E7" s="97">
-        <v>1.0812384259259259E-2</v>
+      <c r="E7" s="97" t="s">
+        <v>198</v>
       </c>
       <c r="F7" s="18" t="s">
         <v>134</v>

</xml_diff>